<commit_message>
this is new code...
</commit_message>
<xml_diff>
--- a/Externaldata/Procurement_Of_Non_Paddy.xlsx
+++ b/Externaldata/Procurement_Of_Non_Paddy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC836BF-D040-4D84-A6BC-96F8FA836544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E83CA07-758F-4A50-8C80-21D7A9A78B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -131,10 +131,7 @@
     <t>PACS Submit status</t>
   </si>
   <si>
-    <t>Successfu</t>
-  </si>
-  <si>
-    <t>Successfully verified</t>
+    <t>Successfully Verified</t>
   </si>
 </sst>
 </file>
@@ -697,7 +694,7 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="5" t="s">

</xml_diff>

<commit_message>
message for this work...
</commit_message>
<xml_diff>
--- a/Externaldata/Procurement_Of_Non_Paddy.xlsx
+++ b/Externaldata/Procurement_Of_Non_Paddy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E83CA07-758F-4A50-8C80-21D7A9A78B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD18658-E578-451C-B955-153BB47BB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -544,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -555,7 +555,7 @@
     <col min="3" max="3" customWidth="true" width="13.44140625"/>
     <col min="4" max="4" customWidth="true" width="20.21875"/>
     <col min="5" max="5" customWidth="true" width="15.21875"/>
-    <col min="6" max="6" customWidth="true" width="14.109375"/>
+    <col min="6" max="6" customWidth="true" width="18.33203125"/>
     <col min="7" max="7" customWidth="true" width="13.88671875"/>
     <col min="8" max="8" customWidth="true" width="17.77734375"/>
     <col min="9" max="9" customWidth="true" width="15.33203125"/>

</xml_diff>

<commit_message>
This is my new code changes
</commit_message>
<xml_diff>
--- a/Externaldata/Procurement_Of_Non_Paddy.xlsx
+++ b/Externaldata/Procurement_Of_Non_Paddy.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD18658-E578-451C-B955-153BB47BB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A5E11-7C32-45AF-84D2-AB7E2CA0DA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -95,12 +95,6 @@
     <t>ADMIN Approved/Rejected status</t>
   </si>
   <si>
-    <t>admin194@gmail.com</t>
-  </si>
-  <si>
-    <t>Cams@1234</t>
-  </si>
-  <si>
     <t>payal@oasys.com</t>
   </si>
   <si>
@@ -110,35 +104,34 @@
     <t>Sashiroul@gmail.com</t>
   </si>
   <si>
-    <t>Abhayapur SCS</t>
-  </si>
-  <si>
-    <t>Ganjam</t>
-  </si>
-  <si>
-    <t>Berhampur</t>
-  </si>
-  <si>
-    <t>Digapahandi</t>
-  </si>
-  <si>
-    <t>Bomakai</t>
-  </si>
-  <si>
     <t>Rama</t>
   </si>
   <si>
     <t>PACS Submit status</t>
   </si>
   <si>
-    <t>Successfully Verified</t>
+    <t>Jharsuguda</t>
+  </si>
+  <si>
+    <t>sasi11@gmail.com</t>
+  </si>
+  <si>
+    <t>Siba@123</t>
+  </si>
+  <si>
+    <t>Laikera</t>
+  </si>
+  <si>
+    <t>LAIKERA SCS</t>
+  </si>
+  <si>
+    <t>Sasi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -544,27 +537,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.0"/>
-    <col min="2" max="2" customWidth="true" width="21.77734375"/>
-    <col min="3" max="3" customWidth="true" width="13.44140625"/>
-    <col min="4" max="4" customWidth="true" width="20.21875"/>
-    <col min="5" max="5" customWidth="true" width="15.21875"/>
-    <col min="6" max="6" customWidth="true" width="18.33203125"/>
-    <col min="7" max="7" customWidth="true" width="13.88671875"/>
-    <col min="8" max="8" customWidth="true" width="17.77734375"/>
-    <col min="9" max="9" customWidth="true" width="15.33203125"/>
-    <col min="10" max="10" customWidth="true" width="18.109375"/>
-    <col min="11" max="11" customWidth="true" width="22.5546875"/>
-    <col min="12" max="12" customWidth="true" width="15.33203125"/>
-    <col min="13" max="13" customWidth="true" width="18.33203125"/>
-    <col min="14" max="14" customWidth="true" width="25.6640625"/>
-    <col min="15" max="15" customWidth="true" width="19.77734375"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
@@ -611,7 +604,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>14</v>
@@ -652,19 +645,19 @@
     </row>
     <row r="2" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>34</v>
@@ -676,7 +669,7 @@
         <v>100</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J2" s="2">
         <v>100</v>
@@ -693,15 +686,12 @@
       <c r="N2" s="2">
         <v>100</v>
       </c>
-      <c r="O2" t="s">
-        <v>38</v>
-      </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -710,10 +700,10 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AA2" s="2"/>
     </row>
@@ -721,6 +711,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="Q2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{6A2CAFE5-00A7-42F7-B6D2-791C531D7B63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>